<commit_message>
New Local_Ks, working on dynamics from spreadsheets
</commit_message>
<xml_diff>
--- a/results/local_calculations_final_state.xlsx
+++ b/results/local_calculations_final_state.xlsx
@@ -1252,9 +1252,7 @@
       <c r="A23" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="35">
-        <v>211.52290249433108</v>
-      </c>
+      <c r="B23" s="35"/>
       <c r="C23" s="35"/>
       <c r="D23" s="36">
         <v>23</v>
@@ -1269,15 +1267,15 @@
       </c>
       <c r="B24" s="11">
         <f>B39</f>
-        <v>2530.5034013605446</v>
+        <v>657.85034013605434</v>
       </c>
       <c r="C24" s="39">
         <f>C39</f>
-        <v>155</v>
+        <v>0</v>
       </c>
       <c r="D24" s="40">
         <f>D39</f>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -1286,15 +1284,15 @@
       </c>
       <c r="B25" s="29">
         <f>SUM(B22:B24)</f>
-        <v>14742.026303854876</v>
+        <v>12657.850340136054</v>
       </c>
       <c r="C25" s="29">
         <f>SUMPRODUCT(C22:C24,$B$22:$B$24)/$B$25</f>
-        <v>121.0300395912554</v>
+        <v>109.97127968768811</v>
       </c>
       <c r="D25" s="30">
         <f>SUMPRODUCT(D22:D24,$B$22:$B$24)/$B$25</f>
-        <v>9.9706130848766907</v>
+        <v>10.428311004866975</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -1309,15 +1307,15 @@
       </c>
       <c r="B27" s="37">
         <f>B19+B25</f>
-        <v>43370.026303854873</v>
+        <v>41285.85034013605</v>
       </c>
       <c r="C27" s="37">
         <f>($B$19*C19+$B$25*C25)/$B$27</f>
-        <v>119.35999279647119</v>
+        <v>115.8851752012681</v>
       </c>
       <c r="D27" s="38">
         <f>($B$19*D19+$B$25*D25)/$B$27</f>
-        <v>9.9900110119209575</v>
+        <v>10.131316093866886</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -1336,7 +1334,7 @@
       </c>
       <c r="D29" s="5">
         <f>SUM(100*(B27-B29)/B29)</f>
-        <v>2.5577763951795243</v>
+        <v>-2.3707069531527805</v>
       </c>
       <c r="E29" t="s">
         <v>30</v>
@@ -1348,7 +1346,7 @@
       </c>
       <c r="B31" s="5">
         <f>B12+B14-D27</f>
-        <v>0.25998898807904247</v>
+        <v>0.11868390613311419</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -1357,7 +1355,7 @@
       </c>
       <c r="B32" s="5">
         <f>B13+B14-D27</f>
-        <v>174.25998898807904</v>
+        <v>174.11868390613313</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1366,7 +1364,7 @@
       </c>
       <c r="B33" s="13">
         <f>(C27-B15)*B7/B32</f>
-        <v>1.1696218618355068</v>
+        <v>-3.5591440470199434</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>47</v>
@@ -1393,18 +1391,14 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="10">
-        <v>2994.6785814917685</v>
+        <v>778.52111258704656</v>
       </c>
       <c r="B39">
         <f>A39*$B$3/1000</f>
-        <v>2530.5034013605446</v>
-      </c>
-      <c r="C39" s="12">
-        <v>155</v>
-      </c>
-      <c r="D39" s="12">
-        <v>4</v>
-      </c>
+        <v>657.85034013605434</v>
+      </c>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
       <c r="E39" t="s">
         <v>32</v>
       </c>

</xml_diff>